<commit_message>
fix a lat of bug
</commit_message>
<xml_diff>
--- a/ITE4116M/Assets/_Excel/card.xlsx
+++ b/ITE4116M/Assets/_Excel/card.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\FYP\ITE4116M\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0019E447-546F-4604-A2A6-3A0B54557E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03200028-403F-4C1E-AFD6-2D4E8E370F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
@@ -55,103 +55,134 @@
     <t>Effects</t>
   </si>
   <si>
+    <t>DefendCard</t>
+  </si>
+  <si>
+    <t>AddCard</t>
+  </si>
+  <si>
+    <t>Icon/RedCard</t>
+  </si>
+  <si>
+    <t>Icon/wood_01a</t>
+  </si>
+  <si>
+    <t>Effects/SmokeExplosionDark</t>
+  </si>
+  <si>
+    <t>Deal {0} points of damage to a single enemy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase {0} shield points</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draw {0} cards from the deck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spurious</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圖示資源的路徑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗的費用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屬性值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌的背景圖資源路徑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌類型的Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌新增的腳本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唯一的識別（不能重複）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>AttackCardItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShieldBash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal {0} points of damage to a single enemy and Increase {0} shield points</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Icon/BlueCard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Icon/sword_03e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Effects/GreenBloodExplosion</t>
-  </si>
-  <si>
-    <t>DefendCard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContinuousAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal {0} points of damage to a single enemy Until the magic power runs out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strongdefense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase {0} shield points Until the magic power runs out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Icon/GreenCard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Icon/armor_01a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Effects/SpinZoneBlue</t>
-  </si>
-  <si>
-    <t>AddCard</t>
-  </si>
-  <si>
-    <t>Icon/RedCard</t>
-  </si>
-  <si>
-    <t>Icon/wood_01a</t>
-  </si>
-  <si>
-    <t>Effects/SmokeExplosionDark</t>
-  </si>
-  <si>
-    <t>Deal {0} points of damage to a single enemy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Increase {0} shield points</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Draw {0} cards from the deck</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Defense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spurious</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>圖示資源的路徑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>消耗的費用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>屬性值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>特效</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌的背景圖資源路徑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌類型的Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌新增的腳本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>唯一的識別（不能重複）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -573,34 +604,34 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -608,31 +639,31 @@
         <v>1000</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D3" s="1">
         <v>10001</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>100</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -640,31 +671,31 @@
         <v>1001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
         <v>10002</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -672,22 +703,22 @@
         <v>1002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>10003</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1">
         <v>2</v>
@@ -696,7 +727,103 @@
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10001</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>40</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10001</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10002</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>